<commit_message>
Many edits to raw data; now working scripts to match fixes to transect sections; in process of checking against GIS.
</commit_message>
<xml_diff>
--- a/data/Raw/Bat Results.xlsx
+++ b/data/Raw/Bat Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>03.09.2014</t>
+  </si>
+  <si>
+    <t>04.09.2014</t>
   </si>
 </sst>
 </file>
@@ -492,11 +495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I550"/>
+  <dimension ref="A1:I579"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H544" sqref="H544"/>
+      <pane ySplit="1" topLeftCell="A561" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E580" sqref="E580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14812,6 +14815,760 @@
         <v>11</v>
       </c>
     </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>33</v>
+      </c>
+      <c r="B551" t="s">
+        <v>44</v>
+      </c>
+      <c r="C551">
+        <v>1</v>
+      </c>
+      <c r="D551" s="2">
+        <v>0</v>
+      </c>
+      <c r="E551" s="1">
+        <v>0.86581018518518515</v>
+      </c>
+      <c r="F551" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G551" s="2">
+        <v>0</v>
+      </c>
+      <c r="H551" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>33</v>
+      </c>
+      <c r="B552" t="s">
+        <v>44</v>
+      </c>
+      <c r="C552">
+        <v>1</v>
+      </c>
+      <c r="D552" s="2">
+        <v>100</v>
+      </c>
+      <c r="E552" s="1">
+        <v>0.86834490740740744</v>
+      </c>
+      <c r="F552" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G552" s="2">
+        <v>0</v>
+      </c>
+      <c r="H552" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>33</v>
+      </c>
+      <c r="B553" t="s">
+        <v>44</v>
+      </c>
+      <c r="C553">
+        <v>1</v>
+      </c>
+      <c r="D553" s="2">
+        <v>200</v>
+      </c>
+      <c r="E553" s="1">
+        <v>0.86996527777777777</v>
+      </c>
+      <c r="F553" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G553" s="2">
+        <v>0</v>
+      </c>
+      <c r="H553" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>33</v>
+      </c>
+      <c r="B554" t="s">
+        <v>44</v>
+      </c>
+      <c r="C554">
+        <v>1</v>
+      </c>
+      <c r="D554" s="2">
+        <v>300</v>
+      </c>
+      <c r="E554" s="1">
+        <v>0.87155092592592587</v>
+      </c>
+      <c r="F554" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G554" s="2">
+        <v>0</v>
+      </c>
+      <c r="H554" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>33</v>
+      </c>
+      <c r="B555" t="s">
+        <v>44</v>
+      </c>
+      <c r="C555">
+        <v>1</v>
+      </c>
+      <c r="D555" s="2">
+        <v>400</v>
+      </c>
+      <c r="E555" s="1">
+        <v>0.87328703703703703</v>
+      </c>
+      <c r="F555" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G555" s="2">
+        <v>0</v>
+      </c>
+      <c r="H555" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>33</v>
+      </c>
+      <c r="B556" t="s">
+        <v>44</v>
+      </c>
+      <c r="C556">
+        <v>1</v>
+      </c>
+      <c r="D556" s="2">
+        <v>500</v>
+      </c>
+      <c r="E556" s="1">
+        <v>0.87510416666666668</v>
+      </c>
+      <c r="F556" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G556" s="2">
+        <v>0</v>
+      </c>
+      <c r="H556" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="557" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>33</v>
+      </c>
+      <c r="B557" t="s">
+        <v>44</v>
+      </c>
+      <c r="C557">
+        <v>1</v>
+      </c>
+      <c r="D557" s="2">
+        <v>600</v>
+      </c>
+      <c r="E557" s="1">
+        <v>0.87699074074074079</v>
+      </c>
+      <c r="F557" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G557" s="2">
+        <v>0</v>
+      </c>
+      <c r="H557" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>33</v>
+      </c>
+      <c r="B558" t="s">
+        <v>44</v>
+      </c>
+      <c r="C558">
+        <v>2</v>
+      </c>
+      <c r="D558" s="2">
+        <v>0</v>
+      </c>
+      <c r="E558" s="1">
+        <v>0.91931712962962964</v>
+      </c>
+      <c r="F558" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G558" s="2">
+        <v>0</v>
+      </c>
+      <c r="H558" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>33</v>
+      </c>
+      <c r="B559" t="s">
+        <v>44</v>
+      </c>
+      <c r="C559">
+        <v>2</v>
+      </c>
+      <c r="D559" s="2">
+        <v>100</v>
+      </c>
+      <c r="E559" s="1">
+        <v>0.92143518518518519</v>
+      </c>
+      <c r="F559" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G559" s="2">
+        <v>0</v>
+      </c>
+      <c r="H559" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="560" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>33</v>
+      </c>
+      <c r="B560" t="s">
+        <v>44</v>
+      </c>
+      <c r="C560">
+        <v>2</v>
+      </c>
+      <c r="D560" s="2">
+        <v>200</v>
+      </c>
+      <c r="E560" s="1">
+        <v>0.92358796296296297</v>
+      </c>
+      <c r="F560" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G560" s="2">
+        <v>0</v>
+      </c>
+      <c r="H560" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="561" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>33</v>
+      </c>
+      <c r="B561" t="s">
+        <v>44</v>
+      </c>
+      <c r="C561">
+        <v>2</v>
+      </c>
+      <c r="D561" s="2">
+        <v>300</v>
+      </c>
+      <c r="E561" s="1">
+        <v>0.92497685185185186</v>
+      </c>
+      <c r="F561" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G561" s="2">
+        <v>0</v>
+      </c>
+      <c r="H561" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="562" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>33</v>
+      </c>
+      <c r="B562" t="s">
+        <v>44</v>
+      </c>
+      <c r="C562">
+        <v>2</v>
+      </c>
+      <c r="D562" s="2">
+        <v>400</v>
+      </c>
+      <c r="E562" s="1">
+        <v>0.9264930555555555</v>
+      </c>
+      <c r="F562" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G562" s="2">
+        <v>0</v>
+      </c>
+      <c r="H562" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>33</v>
+      </c>
+      <c r="B563" t="s">
+        <v>44</v>
+      </c>
+      <c r="C563">
+        <v>2</v>
+      </c>
+      <c r="D563" s="2">
+        <v>500</v>
+      </c>
+      <c r="E563" s="1">
+        <v>0.92791666666666661</v>
+      </c>
+      <c r="F563" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G563" s="2">
+        <v>0</v>
+      </c>
+      <c r="H563" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>33</v>
+      </c>
+      <c r="B564" t="s">
+        <v>44</v>
+      </c>
+      <c r="C564">
+        <v>2</v>
+      </c>
+      <c r="D564" s="2">
+        <v>600</v>
+      </c>
+      <c r="E564" s="1">
+        <v>0.92962962962962958</v>
+      </c>
+      <c r="F564" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G564" s="2">
+        <v>0</v>
+      </c>
+      <c r="H564" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>33</v>
+      </c>
+      <c r="B565" t="s">
+        <v>44</v>
+      </c>
+      <c r="C565">
+        <v>3</v>
+      </c>
+      <c r="D565" s="2">
+        <v>0</v>
+      </c>
+      <c r="E565" s="1">
+        <v>0.90055555555555555</v>
+      </c>
+      <c r="F565" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G565" s="2">
+        <v>0</v>
+      </c>
+      <c r="H565" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>33</v>
+      </c>
+      <c r="B566" t="s">
+        <v>44</v>
+      </c>
+      <c r="C566">
+        <v>3</v>
+      </c>
+      <c r="D566" s="2">
+        <v>100</v>
+      </c>
+      <c r="E566" s="1">
+        <v>0.90312500000000007</v>
+      </c>
+      <c r="F566" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G566" s="2">
+        <v>0</v>
+      </c>
+      <c r="H566" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>33</v>
+      </c>
+      <c r="B567" t="s">
+        <v>44</v>
+      </c>
+      <c r="C567">
+        <v>3</v>
+      </c>
+      <c r="D567" s="2">
+        <v>200</v>
+      </c>
+      <c r="E567" s="1">
+        <v>0.90494212962962972</v>
+      </c>
+      <c r="F567" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G567" s="2">
+        <v>0</v>
+      </c>
+      <c r="H567" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="568" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>33</v>
+      </c>
+      <c r="B568" t="s">
+        <v>44</v>
+      </c>
+      <c r="C568">
+        <v>3</v>
+      </c>
+      <c r="D568" s="2">
+        <v>300</v>
+      </c>
+      <c r="E568" s="1">
+        <v>0.90678240740740745</v>
+      </c>
+      <c r="F568" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G568" s="2">
+        <v>0</v>
+      </c>
+      <c r="H568" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="569" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>33</v>
+      </c>
+      <c r="B569" t="s">
+        <v>44</v>
+      </c>
+      <c r="C569">
+        <v>3</v>
+      </c>
+      <c r="D569" s="2">
+        <v>400</v>
+      </c>
+      <c r="E569" s="1">
+        <v>0.90861111111111104</v>
+      </c>
+      <c r="F569" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G569" s="2">
+        <v>0</v>
+      </c>
+      <c r="H569" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>33</v>
+      </c>
+      <c r="B570" t="s">
+        <v>44</v>
+      </c>
+      <c r="C570">
+        <v>3</v>
+      </c>
+      <c r="D570" s="2">
+        <v>500</v>
+      </c>
+      <c r="E570" s="1">
+        <v>0.91038194444444442</v>
+      </c>
+      <c r="F570" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G570" s="2">
+        <v>0</v>
+      </c>
+      <c r="H570" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>33</v>
+      </c>
+      <c r="B571" t="s">
+        <v>44</v>
+      </c>
+      <c r="C571">
+        <v>3</v>
+      </c>
+      <c r="D571" s="2">
+        <v>600</v>
+      </c>
+      <c r="E571" s="1">
+        <v>0.91200231481481486</v>
+      </c>
+      <c r="F571" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G571" s="2">
+        <v>0</v>
+      </c>
+      <c r="H571" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>33</v>
+      </c>
+      <c r="B572" t="s">
+        <v>44</v>
+      </c>
+      <c r="C572">
+        <v>3</v>
+      </c>
+      <c r="D572" s="2">
+        <v>700</v>
+      </c>
+      <c r="E572" s="1">
+        <v>0.91361111111111104</v>
+      </c>
+      <c r="F572" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G572" s="2">
+        <v>0</v>
+      </c>
+      <c r="H572" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>33</v>
+      </c>
+      <c r="B573" t="s">
+        <v>44</v>
+      </c>
+      <c r="C573">
+        <v>4</v>
+      </c>
+      <c r="D573" s="2">
+        <v>0</v>
+      </c>
+      <c r="E573" s="1">
+        <v>0.88351851851851848</v>
+      </c>
+      <c r="F573" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G573" s="2">
+        <v>0</v>
+      </c>
+      <c r="H573" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>33</v>
+      </c>
+      <c r="B574" t="s">
+        <v>44</v>
+      </c>
+      <c r="C574">
+        <v>4</v>
+      </c>
+      <c r="D574" s="2">
+        <v>100</v>
+      </c>
+      <c r="E574" s="1">
+        <v>0.88615740740740734</v>
+      </c>
+      <c r="F574" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G574" s="2">
+        <v>0</v>
+      </c>
+      <c r="H574" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>33</v>
+      </c>
+      <c r="B575" t="s">
+        <v>44</v>
+      </c>
+      <c r="C575">
+        <v>4</v>
+      </c>
+      <c r="D575" s="2">
+        <v>200</v>
+      </c>
+      <c r="E575" s="1">
+        <v>0.88800925925925922</v>
+      </c>
+      <c r="F575" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G575" s="2">
+        <v>0</v>
+      </c>
+      <c r="H575" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>33</v>
+      </c>
+      <c r="B576" t="s">
+        <v>44</v>
+      </c>
+      <c r="C576">
+        <v>4</v>
+      </c>
+      <c r="D576" s="2">
+        <v>300</v>
+      </c>
+      <c r="E576" s="1">
+        <v>0.88974537037037038</v>
+      </c>
+      <c r="F576" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G576" s="2">
+        <v>0</v>
+      </c>
+      <c r="H576" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>33</v>
+      </c>
+      <c r="B577" t="s">
+        <v>44</v>
+      </c>
+      <c r="C577">
+        <v>4</v>
+      </c>
+      <c r="D577" s="2">
+        <v>400</v>
+      </c>
+      <c r="E577" s="1">
+        <v>0.89134259259259263</v>
+      </c>
+      <c r="F577" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G577" s="2">
+        <v>0</v>
+      </c>
+      <c r="H577" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>33</v>
+      </c>
+      <c r="B578" t="s">
+        <v>44</v>
+      </c>
+      <c r="C578">
+        <v>4</v>
+      </c>
+      <c r="D578" s="2">
+        <v>500</v>
+      </c>
+      <c r="E578" s="1">
+        <v>0.89307870370370368</v>
+      </c>
+      <c r="F578" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G578" s="2">
+        <v>0</v>
+      </c>
+      <c r="H578" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="579" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>33</v>
+      </c>
+      <c r="B579" t="s">
+        <v>44</v>
+      </c>
+      <c r="C579">
+        <v>4</v>
+      </c>
+      <c r="D579" s="2">
+        <v>600</v>
+      </c>
+      <c r="E579" s="1">
+        <v>0.89482638888888888</v>
+      </c>
+      <c r="F579" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="G579" s="2">
+        <v>0</v>
+      </c>
+      <c r="H579" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>